<commit_message>
each.with_index -> each_with_index todo: optimize writing data to db
</commit_message>
<xml_diff>
--- a/test/fixtures/files/NguyenHuynhThanhThao-Review cheo.Dinh tinh.xlsx
+++ b/test/fixtures/files/NguyenHuynhThanhThao-Review cheo.Dinh tinh.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="考え方- Tu duy" sheetId="1" r:id="rId1"/>
-    <sheet name="熱意- Nhiet tinh" sheetId="2" r:id="rId2"/>
-    <sheet name="Vai trò -Chung " sheetId="9" r:id="rId3"/>
-    <sheet name="Vai trò -Leader" sheetId="10" r:id="rId4"/>
-    <sheet name="Vai trò -Manager" sheetId="11" r:id="rId5"/>
+    <sheet name="考え方- tu_duy" sheetId="1" r:id="rId1"/>
+    <sheet name="熱意- nhiet_tinh" sheetId="2" r:id="rId2"/>
+    <sheet name="chung- vai_tro " sheetId="9" r:id="rId3"/>
+    <sheet name="leader- vai_tro" sheetId="10" r:id="rId4"/>
+    <sheet name="manager- vai_tro" sheetId="11" r:id="rId5"/>
     <sheet name="能力" sheetId="3" state="hidden" r:id="rId6"/>
     <sheet name="スキル2.0" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
@@ -4360,26 +4360,6 @@
     </r>
   </si>
   <si>
-    <t>レビュー
-Review- Tri</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Lệ</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Long</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Nhu</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Thịnh</t>
-  </si>
-  <si>
     <t>Leader</t>
   </si>
   <si>
@@ -4455,10 +4435,6 @@
   <si>
     <t>Làm rõ các KPI, phân tích chúng hàng tuần, thông báo cho nhóm và quản lý cấp cao,
  đồng thời nâng cao mức hoạt động cần thiết</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Linh</t>
   </si>
   <si>
     <t>Khởi điểm</t>
@@ -4546,43 +4522,7 @@
 mà còn với các đối tác kinh doanh và các nhóm ngành.</t>
   </si>
   <si>
-    <t>レビュー
-Review- anh Lâm</t>
-  </si>
-  <si>
     <t>Note: Thực hiện đánh giá khách quan cho tất cả mọi người. Bỏ trống phần có tên của chính mình.</t>
-  </si>
-  <si>
-    <t>レビュー
-Review-anh Lâm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">レビュー
-Review- Tài </t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Đạt</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Dũng</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Nam</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Khương</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Tài</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Thuận</t>
   </si>
   <si>
     <t>レビュー
@@ -4593,19 +4533,79 @@
   </si>
   <si>
     <t>レビュー
-Review- Thảo(nữ)</t>
+Review- DangThanhLam</t>
   </si>
   <si>
     <t>レビュー
-Review- Tuấn Anh</t>
+Review- NguyenMinhTri</t>
   </si>
   <si>
     <t>レビュー
-Review- Thảo (nam)</t>
+Review- TranPhatTai</t>
   </si>
   <si>
     <t>レビュー
-Review- Minh</t>
+Review- DangPhatThinh</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- LeThiThuyLinh</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenThiNhatLe</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- LeMinhLong</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- DangHoangNhu</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- TranTienDat</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- DinHienDung</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- MaiNhatNam</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenLeKhuong</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- TranKhanhThuan</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenHuynhThanhThao</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- PhamTuanAnh</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenVanThao</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenQuangMinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">レビュー
+Review- TranPhatTai </t>
+  </si>
+  <si>
+    <t>レビュー
+Review-DangThanhLam</t>
   </si>
 </sst>
 </file>
@@ -5209,8 +5209,11 @@
     <xf numFmtId="0" fontId="27" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5218,11 +5221,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5530,7 +5530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5543,11 +5543,11 @@
   </sheetPr>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5557,7 +5557,9 @@
     <col min="3" max="3" width="78.85546875" style="11" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="20" max="20" width="24.85546875" customWidth="1"/>
     <col min="21" max="21" width="8.7109375" style="44" customWidth="1"/>
     <col min="22" max="22" width="10.28515625" customWidth="1"/>
     <col min="23" max="23" width="9.85546875" customWidth="1"/>
@@ -5570,71 +5572,71 @@
       <c r="B1" s="14"/>
       <c r="C1"/>
       <c r="D1" s="43" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="F1" s="43"/>
     </row>
-    <row r="2" spans="1:23" s="36" customFormat="1" ht="78.75">
+    <row r="2" spans="1:23" s="36" customFormat="1" ht="94.5">
       <c r="C2" s="37"/>
       <c r="D2" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="F2" s="38" t="s">
+      <c r="H2" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="O2" s="38" t="s">
         <v>337</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>282</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>333</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>336</v>
       </c>
       <c r="P2" s="38" t="s">
         <v>338</v>
       </c>
       <c r="Q2" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="S2" s="38" t="s">
         <v>341</v>
       </c>
-      <c r="R2" s="38" t="s">
+      <c r="T2" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="S2" s="38" t="s">
-        <v>343</v>
-      </c>
-      <c r="T2" s="38" t="s">
-        <v>344</v>
-      </c>
       <c r="U2" s="45" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="V2" s="46" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="W2" s="46" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="24">
@@ -7519,10 +7521,10 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3:U27"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7546,72 +7548,72 @@
         <v>208</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
     </row>
-    <row r="2" spans="1:24" s="36" customFormat="1" ht="78.75">
+    <row r="2" spans="1:24" s="36" customFormat="1" ht="94.5">
       <c r="C2" s="37"/>
       <c r="E2" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="F2" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="G2" s="38" t="s">
+      <c r="I2" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="P2" s="38" t="s">
         <v>337</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>282</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>333</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>336</v>
       </c>
       <c r="Q2" s="38" t="s">
         <v>338</v>
       </c>
       <c r="R2" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="T2" s="38" t="s">
         <v>341</v>
       </c>
-      <c r="S2" s="38" t="s">
+      <c r="U2" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="T2" s="38" t="s">
-        <v>343</v>
-      </c>
-      <c r="U2" s="38" t="s">
-        <v>344</v>
-      </c>
       <c r="V2" s="45" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="W2" s="46" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="X2" s="46" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="24">
@@ -7621,10 +7623,10 @@
       <c r="B3" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="54"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="30">
         <v>4</v>
       </c>
@@ -7693,10 +7695,10 @@
       <c r="B4" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="54" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="30">
         <v>5</v>
       </c>
@@ -7765,10 +7767,10 @@
       <c r="B5" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="30">
         <v>5</v>
       </c>
@@ -7837,10 +7839,10 @@
       <c r="B6" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="30">
         <v>3</v>
       </c>
@@ -7909,10 +7911,10 @@
       <c r="B7" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="54"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="30">
         <v>3</v>
       </c>
@@ -7981,10 +7983,10 @@
       <c r="B8" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="D8" s="54"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="30">
         <v>5</v>
       </c>
@@ -8053,10 +8055,10 @@
       <c r="B9" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="D9" s="56"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="30">
         <v>5</v>
       </c>
@@ -8125,10 +8127,10 @@
       <c r="B10" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="30">
         <v>4</v>
       </c>
@@ -8197,10 +8199,10 @@
       <c r="B11" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="30">
         <v>4</v>
       </c>
@@ -8269,10 +8271,10 @@
       <c r="B12" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="54" t="s">
         <v>220</v>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="30">
         <v>5</v>
       </c>
@@ -8341,10 +8343,10 @@
       <c r="B13" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="D13" s="54"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="30">
         <v>5</v>
       </c>
@@ -8413,10 +8415,10 @@
       <c r="B14" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="D14" s="54"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="30">
         <v>3</v>
       </c>
@@ -8485,10 +8487,10 @@
       <c r="B15" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="54" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="54"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="30">
         <v>3</v>
       </c>
@@ -8557,10 +8559,10 @@
       <c r="B16" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="54" t="s">
         <v>227</v>
       </c>
-      <c r="D16" s="54"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="30">
         <v>5</v>
       </c>
@@ -8629,10 +8631,10 @@
       <c r="B17" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="54" t="s">
         <v>228</v>
       </c>
-      <c r="D17" s="54"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="30">
         <v>3</v>
       </c>
@@ -8701,10 +8703,10 @@
       <c r="B18" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="54"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="30">
         <v>4</v>
       </c>
@@ -8773,10 +8775,10 @@
       <c r="B19" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="D19" s="54"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="30">
         <v>4</v>
       </c>
@@ -8845,10 +8847,10 @@
       <c r="B20" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="54" t="s">
         <v>231</v>
       </c>
-      <c r="D20" s="54"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="30">
         <v>5</v>
       </c>
@@ -8917,10 +8919,10 @@
       <c r="B21" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="54" t="s">
         <v>232</v>
       </c>
-      <c r="D21" s="54"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="30">
         <v>4</v>
       </c>
@@ -8989,10 +8991,10 @@
       <c r="B22" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="54" t="s">
         <v>233</v>
       </c>
-      <c r="D22" s="54"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="30">
         <v>4</v>
       </c>
@@ -9061,10 +9063,10 @@
       <c r="B23" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="D23" s="54"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="30">
         <v>4</v>
       </c>
@@ -9133,10 +9135,10 @@
       <c r="B24" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="D24" s="56"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="30">
         <v>4</v>
       </c>
@@ -9204,10 +9206,10 @@
       <c r="B25" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="D25" s="56"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="30">
         <v>5</v>
       </c>
@@ -9275,10 +9277,10 @@
       <c r="B26" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C26" s="53" t="s">
+      <c r="C26" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="D26" s="54"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="30">
         <v>5</v>
       </c>
@@ -9346,10 +9348,10 @@
       <c r="B27" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="52" t="s">
         <v>238</v>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="30">
         <v>5</v>
       </c>
@@ -9514,54 +9516,71 @@
       <c r="B32" s="1">
         <v>4</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="D32" s="52"/>
+      <c r="D32" s="56"/>
       <c r="E32" s="12"/>
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1">
       <c r="B33" s="1">
         <v>3</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="56" t="s">
         <v>241</v>
       </c>
-      <c r="D33" s="52"/>
+      <c r="D33" s="56"/>
       <c r="E33" s="12"/>
     </row>
     <row r="34" spans="2:5" ht="31.5" customHeight="1">
       <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C34" s="52" t="s">
+      <c r="C34" s="56" t="s">
         <v>242</v>
       </c>
-      <c r="D34" s="52"/>
+      <c r="D34" s="56"/>
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="2:5" ht="39" customHeight="1">
       <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="D35" s="52"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="12"/>
     </row>
     <row r="36" spans="2:5" ht="36.75" customHeight="1">
       <c r="B36" s="1">
         <v>0</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="D36" s="52"/>
+      <c r="D36" s="56"/>
       <c r="E36" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C3:D3"/>
@@ -9578,23 +9597,6 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -9610,10 +9612,10 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9636,70 +9638,70 @@
         <v>246</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="36" customFormat="1" ht="78.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="36" customFormat="1" ht="94.5">
       <c r="C2" s="37"/>
       <c r="E2" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="F2" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="G2" s="38" t="s">
+      <c r="I2" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="P2" s="38" t="s">
         <v>337</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>282</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>333</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>336</v>
       </c>
       <c r="Q2" s="38" t="s">
         <v>338</v>
       </c>
       <c r="R2" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="T2" s="38" t="s">
         <v>341</v>
       </c>
-      <c r="S2" s="38" t="s">
+      <c r="U2" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="T2" s="38" t="s">
-        <v>343</v>
-      </c>
-      <c r="U2" s="38" t="s">
-        <v>344</v>
-      </c>
       <c r="V2" s="45" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="W2" s="46" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="X2" s="46" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="27" customFormat="1" ht="31.5">
@@ -11245,7 +11247,7 @@
     <row r="24" spans="1:24">
       <c r="V24"/>
       <c r="X24" s="49">
-        <f>X23+'熱意- Nhiet tinh'!X28+'考え方- Tu duy'!W28</f>
+        <f>X23+'熱意- nhiet_tinh'!X28+'考え方- tu_duy'!W28</f>
         <v>439.15</v>
       </c>
     </row>
@@ -11344,7 +11346,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11364,20 +11366,20 @@
         <v>246</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="31.5">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="63">
       <c r="E2" s="38" t="s">
-        <v>280</v>
+        <v>327</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="27" customFormat="1" ht="15.75">
       <c r="A3" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>248</v>
@@ -11386,7 +11388,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E3" s="33">
         <v>4</v>
@@ -11397,7 +11399,7 @@
     </row>
     <row r="4" spans="1:6" s="27" customFormat="1" ht="29.1" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>248</v>
@@ -11406,7 +11408,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E4" s="33">
         <v>2</v>
@@ -11417,7 +11419,7 @@
     </row>
     <row r="5" spans="1:6" s="27" customFormat="1" ht="29.1" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>248</v>
@@ -11426,7 +11428,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E5" s="33">
         <v>4</v>
@@ -11437,7 +11439,7 @@
     </row>
     <row r="6" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A6" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>248</v>
@@ -11446,7 +11448,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E6" s="33">
         <v>2</v>
@@ -11457,7 +11459,7 @@
     </row>
     <row r="7" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A7" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>248</v>
@@ -11466,7 +11468,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E7" s="33">
         <v>4</v>
@@ -11477,7 +11479,7 @@
     </row>
     <row r="8" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A8" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>248</v>
@@ -11486,7 +11488,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E8" s="33">
         <v>2</v>
@@ -11497,7 +11499,7 @@
     </row>
     <row r="9" spans="1:6" s="27" customFormat="1" ht="24.95" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>248</v>
@@ -11506,7 +11508,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E9" s="33">
         <v>4</v>
@@ -11517,7 +11519,7 @@
     </row>
     <row r="10" spans="1:6" s="27" customFormat="1" ht="15.75">
       <c r="A10" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>248</v>
@@ -11526,7 +11528,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E10" s="33">
         <v>3</v>
@@ -11537,7 +11539,7 @@
     </row>
     <row r="11" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A11" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>248</v>
@@ -11546,7 +11548,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E11" s="33">
         <v>3</v>
@@ -11557,7 +11559,7 @@
     </row>
     <row r="12" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A12" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>248</v>
@@ -11566,7 +11568,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E12" s="33">
         <v>4</v>
@@ -11577,7 +11579,7 @@
     </row>
     <row r="13" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A13" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>248</v>
@@ -11586,7 +11588,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E13" s="33">
         <v>3</v>
@@ -11597,7 +11599,7 @@
     </row>
     <row r="14" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A14" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>248</v>
@@ -11606,7 +11608,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E14" s="33">
         <v>4</v>
@@ -11617,7 +11619,7 @@
     </row>
     <row r="15" spans="1:6" s="27" customFormat="1" ht="15.75">
       <c r="A15" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>248</v>
@@ -11626,7 +11628,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E15" s="33">
         <v>2</v>
@@ -11637,7 +11639,7 @@
     </row>
     <row r="16" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A16" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>248</v>
@@ -11646,7 +11648,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E16" s="33">
         <v>4</v>
@@ -11657,7 +11659,7 @@
     </row>
     <row r="17" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A17" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>248</v>
@@ -11666,7 +11668,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E17" s="33">
         <v>4</v>
@@ -11677,7 +11679,7 @@
     </row>
     <row r="18" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A18" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>248</v>
@@ -11686,7 +11688,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E18" s="33">
         <v>2</v>
@@ -11697,7 +11699,7 @@
     </row>
     <row r="19" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A19" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>248</v>
@@ -11706,7 +11708,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E19" s="33">
         <v>3</v>
@@ -11717,7 +11719,7 @@
     </row>
     <row r="20" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A20" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>248</v>
@@ -11726,7 +11728,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E20" s="33">
         <v>2</v>
@@ -11737,7 +11739,7 @@
     </row>
     <row r="21" spans="1:6" s="27" customFormat="1" ht="15.75">
       <c r="A21" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>248</v>
@@ -11746,7 +11748,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E21" s="33">
         <v>3</v>
@@ -11757,7 +11759,7 @@
     </row>
     <row r="22" spans="1:6" s="27" customFormat="1" ht="31.5">
       <c r="A22" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>248</v>
@@ -11766,7 +11768,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E22" s="33">
         <v>3</v>
@@ -11876,11 +11878,11 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11901,23 +11903,23 @@
         <v>246</v>
       </c>
       <c r="E1" s="43" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="63">
+      <c r="E2" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="47.25">
-      <c r="E2" s="38" t="s">
-        <v>331</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A3" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>248</v>
@@ -11926,7 +11928,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E3" s="41">
         <v>3</v>
@@ -11938,7 +11940,7 @@
     </row>
     <row r="4" spans="1:7" s="27" customFormat="1" ht="29.1" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>248</v>
@@ -11947,7 +11949,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E4" s="41">
         <v>3</v>
@@ -11959,7 +11961,7 @@
     </row>
     <row r="5" spans="1:7" s="27" customFormat="1" ht="29.1" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>248</v>
@@ -11968,7 +11970,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E5" s="41">
         <v>4</v>
@@ -11980,7 +11982,7 @@
     </row>
     <row r="6" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A6" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>248</v>
@@ -11989,7 +11991,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E6" s="41">
         <v>4</v>
@@ -12001,7 +12003,7 @@
     </row>
     <row r="7" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A7" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>248</v>
@@ -12010,7 +12012,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E7" s="41">
         <v>3</v>
@@ -12022,7 +12024,7 @@
     </row>
     <row r="8" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A8" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>248</v>
@@ -12031,7 +12033,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E8" s="41">
         <v>3</v>
@@ -12043,7 +12045,7 @@
     </row>
     <row r="9" spans="1:7" s="27" customFormat="1" ht="33.6" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>248</v>
@@ -12052,7 +12054,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E9" s="41">
         <v>4</v>
@@ -12064,7 +12066,7 @@
     </row>
     <row r="10" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A10" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>248</v>
@@ -12073,7 +12075,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E10" s="41">
         <v>4</v>
@@ -12085,7 +12087,7 @@
     </row>
     <row r="11" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A11" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>248</v>
@@ -12094,7 +12096,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E11" s="41">
         <v>3</v>
@@ -12106,7 +12108,7 @@
     </row>
     <row r="12" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A12" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>248</v>
@@ -12115,7 +12117,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E12" s="41">
         <v>4</v>
@@ -12127,7 +12129,7 @@
     </row>
     <row r="13" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A13" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>248</v>
@@ -12136,7 +12138,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E13" s="41">
         <v>4</v>
@@ -12148,7 +12150,7 @@
     </row>
     <row r="14" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A14" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>248</v>
@@ -12157,7 +12159,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E14" s="41">
         <v>3</v>
@@ -12169,7 +12171,7 @@
     </row>
     <row r="15" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A15" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>248</v>
@@ -12178,7 +12180,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E15" s="41">
         <v>4</v>
@@ -12190,7 +12192,7 @@
     </row>
     <row r="16" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A16" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>248</v>
@@ -12199,7 +12201,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E16" s="41">
         <v>4</v>
@@ -12211,7 +12213,7 @@
     </row>
     <row r="17" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A17" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>248</v>
@@ -12220,7 +12222,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E17" s="41">
         <v>3</v>
@@ -12232,7 +12234,7 @@
     </row>
     <row r="18" spans="1:7" s="27" customFormat="1" ht="15.75">
       <c r="A18" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>248</v>
@@ -12241,7 +12243,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E18" s="41">
         <v>3</v>
@@ -12253,7 +12255,7 @@
     </row>
     <row r="19" spans="1:7" s="27" customFormat="1" ht="47.1" customHeight="1">
       <c r="A19" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>248</v>
@@ -12262,7 +12264,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="E19" s="41">
         <v>3</v>
@@ -12274,7 +12276,7 @@
     </row>
     <row r="20" spans="1:7" s="27" customFormat="1" ht="15.75">
       <c r="A20" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>248</v>
@@ -12283,7 +12285,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E20" s="41">
         <v>4</v>
@@ -12295,7 +12297,7 @@
     </row>
     <row r="21" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A21" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>248</v>
@@ -12304,7 +12306,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E21" s="41">
         <v>3</v>
@@ -12316,7 +12318,7 @@
     </row>
     <row r="22" spans="1:7" s="27" customFormat="1" ht="31.5">
       <c r="A22" s="26" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>248</v>
@@ -12325,7 +12327,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E22" s="41">
         <v>3</v>

</xml_diff>